<commit_message>
carga egreso, infractorcontraventor y titular
</commit_message>
<xml_diff>
--- a/Excel/Carga DB Postgres/Egreso - cargado.xlsx
+++ b/Excel/Carga DB Postgres/Egreso - cargado.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="95">
   <si>
     <t>idegreso</t>
   </si>
@@ -289,6 +289,18 @@
   </si>
   <si>
     <t>2017-01-28-18:35:26</t>
+  </si>
+  <si>
+    <t>DNI</t>
+  </si>
+  <si>
+    <t>LE</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>EXT</t>
   </si>
 </sst>
 </file>
@@ -623,7 +635,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -700,8 +712,8 @@
       <c r="J2">
         <v>1</v>
       </c>
-      <c r="K2">
-        <v>1</v>
+      <c r="K2" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -735,8 +747,8 @@
       <c r="J3">
         <v>2</v>
       </c>
-      <c r="K3">
-        <v>2</v>
+      <c r="K3" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -770,8 +782,8 @@
       <c r="J4">
         <v>3</v>
       </c>
-      <c r="K4">
-        <v>3</v>
+      <c r="K4" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -805,8 +817,8 @@
       <c r="J5">
         <v>4</v>
       </c>
-      <c r="K5">
-        <v>2</v>
+      <c r="K5" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -840,8 +852,8 @@
       <c r="J6">
         <v>5</v>
       </c>
-      <c r="K6">
-        <v>1</v>
+      <c r="K6" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -875,8 +887,8 @@
       <c r="J7">
         <v>26</v>
       </c>
-      <c r="K7">
-        <v>4</v>
+      <c r="K7" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -910,8 +922,8 @@
       <c r="J8">
         <v>27</v>
       </c>
-      <c r="K8">
-        <v>2</v>
+      <c r="K8" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -945,8 +957,8 @@
       <c r="J9">
         <v>28</v>
       </c>
-      <c r="K9">
-        <v>3</v>
+      <c r="K9" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -980,8 +992,8 @@
       <c r="J10">
         <v>29</v>
       </c>
-      <c r="K10">
-        <v>1</v>
+      <c r="K10" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1015,8 +1027,8 @@
       <c r="J11">
         <v>30</v>
       </c>
-      <c r="K11">
-        <v>4</v>
+      <c r="K11" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1050,8 +1062,8 @@
       <c r="J12">
         <v>51</v>
       </c>
-      <c r="K12">
-        <v>2</v>
+      <c r="K12" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1085,8 +1097,8 @@
       <c r="J13">
         <v>52</v>
       </c>
-      <c r="K13">
-        <v>3</v>
+      <c r="K13" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1120,8 +1132,8 @@
       <c r="J14">
         <v>53</v>
       </c>
-      <c r="K14">
-        <v>1</v>
+      <c r="K14" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1155,8 +1167,8 @@
       <c r="J15">
         <v>54</v>
       </c>
-      <c r="K15">
-        <v>4</v>
+      <c r="K15" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1190,8 +1202,8 @@
       <c r="J16">
         <v>55</v>
       </c>
-      <c r="K16">
-        <v>2</v>
+      <c r="K16" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1225,8 +1237,8 @@
       <c r="J17">
         <v>86</v>
       </c>
-      <c r="K17">
-        <v>2</v>
+      <c r="K17" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1260,8 +1272,8 @@
       <c r="J18">
         <v>87</v>
       </c>
-      <c r="K18">
-        <v>3</v>
+      <c r="K18" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1295,8 +1307,8 @@
       <c r="J19">
         <v>88</v>
       </c>
-      <c r="K19">
-        <v>1</v>
+      <c r="K19" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1330,8 +1342,8 @@
       <c r="J20">
         <v>89</v>
       </c>
-      <c r="K20">
-        <v>1</v>
+      <c r="K20" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1365,8 +1377,8 @@
       <c r="J21">
         <v>90</v>
       </c>
-      <c r="K21">
-        <v>1</v>
+      <c r="K21" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
carga documento, ingreso, egreso
</commit_message>
<xml_diff>
--- a/Excel/Carga DB Postgres/Egreso - cargado.xlsx
+++ b/Excel/Carga DB Postgres/Egreso - cargado.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" calcMode="manual"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="96">
   <si>
     <t>fechahora</t>
   </si>
@@ -298,6 +298,12 @@
   </si>
   <si>
     <t>EXT</t>
+  </si>
+  <si>
+    <t>2017-11-07-20:00:00</t>
+  </si>
+  <si>
+    <t>2017-11-07-20:00:10</t>
   </si>
 </sst>
 </file>
@@ -629,10 +635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1312,6 +1318,70 @@
         <v>90</v>
       </c>
       <c r="J21" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22">
+        <v>32314054</v>
+      </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" t="s">
+        <v>69</v>
+      </c>
+      <c r="G22" t="s">
+        <v>69</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
+      <c r="I22">
+        <v>121</v>
+      </c>
+      <c r="J22" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23">
+        <v>25745226</v>
+      </c>
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" t="s">
+        <v>51</v>
+      </c>
+      <c r="F23" t="s">
+        <v>69</v>
+      </c>
+      <c r="G23" t="s">
+        <v>69</v>
+      </c>
+      <c r="H23">
+        <v>3</v>
+      </c>
+      <c r="I23">
+        <v>122</v>
+      </c>
+      <c r="J23" t="s">
         <v>90</v>
       </c>
     </row>

</xml_diff>